<commit_message>
removing MAP trees from uncoverged run
</commit_message>
<xml_diff>
--- a/data/cystopteridaceae/20200810_vettingCopyNumber_again/copiesPerLocus.xlsx
+++ b/data/cystopteridaceae/20200810_vettingCopyNumber_again/copiesPerLocus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlrothfels/Box Sync/R_Python_etal/git_repositories/homologizer/data/cystopteridaceae/20200810_vettingCopyNumber_again/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259EBF4B-A06B-424D-A5F1-BBA05343B31C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4FFEE16-63CA-884B-89D8-BC82434AABD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="2160" windowWidth="22060" windowHeight="17000" xr2:uid="{AE534D98-65A7-4D43-BDD4-51ADCD2EEBC6}"/>
   </bookViews>
@@ -659,8 +659,8 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F48" sqref="F48"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
renaming the cystopteridaceae sequence names etc
</commit_message>
<xml_diff>
--- a/data/cystopteridaceae/20200810_vettingCopyNumber_again/copiesPerLocus.xlsx
+++ b/data/cystopteridaceae/20200810_vettingCopyNumber_again/copiesPerLocus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlrothfels/Box Sync/R_Python_etal/git_repositories/homologizer/data/cystopteridaceae/20200810_vettingCopyNumber_again/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3810E3-63E0-AB42-BCCA-2C8442E762D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1C4F11-9DF4-0B45-B84D-EC662794D876}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="22060" windowHeight="17000" xr2:uid="{AE534D98-65A7-4D43-BDD4-51ADCD2EEBC6}"/>
+    <workbookView xWindow="14680" yWindow="460" windowWidth="22060" windowHeight="17000" xr2:uid="{AE534D98-65A7-4D43-BDD4-51ADCD2EEBC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -247,9 +247,6 @@
     <t>The GAP ones look like they might be allelic, rather than homeologs -- create a new tip?</t>
   </si>
   <si>
-    <t>CJRversion of script</t>
-  </si>
-  <si>
     <t>Fixed this, so that this accession is treated as two diploid individuals</t>
   </si>
   <si>
@@ -290,6 +287,9 @@
   </si>
   <si>
     <t>see whether it might be justified to try this one with three tips instead of four</t>
+  </si>
+  <si>
+    <t>v1 script</t>
   </si>
 </sst>
 </file>
@@ -665,8 +665,8 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I42" sqref="I42"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -693,26 +693,26 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" t="s">
         <v>69</v>
       </c>
-      <c r="G1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K1" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
@@ -772,7 +772,7 @@
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
@@ -863,7 +863,7 @@
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
@@ -880,7 +880,7 @@
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
@@ -910,10 +910,10 @@
         <v>59</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -933,7 +933,7 @@
         <v>59</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1014,7 +1014,7 @@
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B18" t="s">
@@ -1074,7 +1074,7 @@
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B21" t="s">
@@ -1134,7 +1134,7 @@
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B24" t="s">
@@ -1150,17 +1150,17 @@
         <v>5</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B25" t="s">
@@ -1170,13 +1170,13 @@
         <v>5</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1242,7 +1242,7 @@
         <v>63</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J28" s="2"/>
     </row>
@@ -1266,7 +1266,7 @@
         <v>63</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J29" s="2"/>
     </row>
@@ -1342,7 +1342,7 @@
       </c>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B34" t="s">
@@ -1418,7 +1418,7 @@
         <v>5</v>
       </c>
       <c r="F37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -1432,7 +1432,7 @@
         <v>5</v>
       </c>
       <c r="F38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -1455,7 +1455,7 @@
         <v>61</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -1495,7 +1495,7 @@
       <c r="J41" s="2"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B42" t="s">
@@ -1511,11 +1511,11 @@
         <v>5</v>
       </c>
       <c r="F42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" t="s">
+      <c r="A43" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D43" t="s">
@@ -1525,7 +1525,7 @@
         <v>5</v>
       </c>
       <c r="F43" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:10">

</xml_diff>